<commit_message>
Cập nhật bài học
</commit_message>
<xml_diff>
--- a/LESSON/HT02.xlsx
+++ b/LESSON/HT02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndmnh\Desktop\Japanese\LESSON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bb3dcffef2d668f/Documents/GitHub/my-pwa/Tieng-Nhat/LESSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{712E1160-D660-4D12-9739-FC7BA566A15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{712E1160-D660-4D12-9739-FC7BA566A15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BF7D871-1A87-4D52-B485-CC3C82FBEB5F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="336" windowWidth="22992" windowHeight="11904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="336" windowWidth="17196" windowHeight="11904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>

</xml_diff>